<commit_message>
Usando un provider en excel haciendo pruebas con selenium y creando el pdf en capturas
</commit_message>
<xml_diff>
--- a/provider/Prueba.xlsx
+++ b/provider/Prueba.xlsx
@@ -19,123 +19,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
-  <si>
-    <t>userName</t>
-  </si>
-  <si>
-    <t>pass</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>TestPass</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Test1</t>
   </si>
   <si>
-    <t>TestPass1</t>
-  </si>
-  <si>
-    <t>FechaTest</t>
-  </si>
-  <si>
-    <t>FechaTest1</t>
-  </si>
-  <si>
     <t>Test2</t>
   </si>
   <si>
-    <t>TestPass2</t>
-  </si>
-  <si>
-    <t>FechaTest2</t>
-  </si>
-  <si>
     <t>Test3</t>
   </si>
   <si>
-    <t>TestPass3</t>
-  </si>
-  <si>
-    <t>FechaTest3</t>
-  </si>
-  <si>
     <t>Test4</t>
   </si>
   <si>
-    <t>TestPass4</t>
-  </si>
-  <si>
-    <t>FechaTest4</t>
-  </si>
-  <si>
     <t>Test5</t>
   </si>
   <si>
-    <t>TestPass5</t>
-  </si>
-  <si>
-    <t>FechaTest5</t>
-  </si>
-  <si>
     <t>Test6</t>
   </si>
   <si>
-    <t>TestPass6</t>
-  </si>
-  <si>
-    <t>FechaTest6</t>
-  </si>
-  <si>
     <t>Test7</t>
   </si>
   <si>
-    <t>TestPass7</t>
-  </si>
-  <si>
-    <t>FechaTest7</t>
-  </si>
-  <si>
     <t>Test8</t>
   </si>
   <si>
-    <t>TestPass8</t>
-  </si>
-  <si>
-    <t>FechaTest8</t>
-  </si>
-  <si>
     <t>Test9</t>
   </si>
   <si>
-    <t>TestPass9</t>
-  </si>
-  <si>
-    <t>FechaTest9</t>
-  </si>
-  <si>
     <t>Test10</t>
   </si>
   <si>
-    <t>TestPass10</t>
-  </si>
-  <si>
-    <t>FechaTest10</t>
-  </si>
-  <si>
     <t>Test11</t>
   </si>
   <si>
-    <t>TestPass11</t>
-  </si>
-  <si>
-    <t>FechaTest11</t>
-  </si>
-  <si>
-    <t>fechaaa</t>
+    <t>Test0</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -454,160 +376,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambiando el webdriver a edge
</commit_message>
<xml_diff>
--- a/provider/Prueba.xlsx
+++ b/provider/Prueba.xlsx
@@ -19,7 +19,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Test0</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
   <si>
     <t>Test1</t>
   </si>
@@ -31,15 +37,6 @@
   </si>
   <si>
     <t>Test4</t>
-  </si>
-  <si>
-    <t>Test5</t>
-  </si>
-  <si>
-    <t>Test0</t>
-  </si>
-  <si>
-    <t>test</t>
   </si>
 </sst>
 </file>
@@ -75,9 +72,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -373,37 +369,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
+      <c r="A3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>